<commit_message>
fields.xlsx: Minor edits to fields list
</commit_message>
<xml_diff>
--- a/fields.xlsx
+++ b/fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jboyk\code_stuff\python\arc_pro_scripting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28AD6CC4-891B-4105-889C-132E460BA01D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BAE215-5BE1-40A4-946E-638AD68C30D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{DEE38724-B8D4-42A6-BA61-437BC0757DB9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="77">
   <si>
     <t>Link_Base</t>
   </si>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t>Label</t>
+  </si>
+  <si>
+    <t># Don't Forgot to remove the last comma</t>
   </si>
 </sst>
 </file>
@@ -632,11 +635,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE6128EF-1ED2-4F71-B387-64DA09F2CECF}">
-  <dimension ref="A1:X43"/>
+  <dimension ref="A1:X44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U35" sqref="U35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,7 +883,7 @@
         <v>61</v>
       </c>
       <c r="W5" t="str">
-        <f t="shared" ref="W5:W43" si="1">CONCATENATE(B5,C5,D5,E5,F5,G5,H5,I5,J5,K5,L5,M5,N5,O5,P5,Q5,R5,S5,T5)</f>
+        <f t="shared" ref="W5:W44" si="1">CONCATENATE(B5,C5,D5,E5,F5,G5,H5,I5,J5,K5,L5,M5,N5,O5,P5,Q5,R5,S5,T5)</f>
         <v>("Link_Part", "String", None, None, None, None, "NULLABLE", None, None),</v>
       </c>
     </row>
@@ -3276,6 +3279,15 @@
       <c r="W43" t="str">
         <f t="shared" si="1"/>
         <v>("Shape_Area", "Double", None, None, None, None, "NULLABLE", None, None),</v>
+      </c>
+    </row>
+    <row r="44" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>76</v>
+      </c>
+      <c r="W44" t="str">
+        <f t="shared" si="1"/>
+        <v># Don't Forgot to remove the last comma</v>
       </c>
     </row>
   </sheetData>

</xml_diff>